<commit_message>
Integrado en la aplicación móvil, retocados los estilos para que header y footer sean estáticos y metida transición entre pantallas para dar efecto de app nativa.
</commit_message>
<xml_diff>
--- a/documentacion/Documentacion_final/11 Registro de Incidencias_RI.xlsx
+++ b/documentacion/Documentacion_final/11 Registro de Incidencias_RI.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>001</t>
   </si>
@@ -170,6 +170,30 @@
   </si>
   <si>
     <t>Se cambia de plugin cordova para que funcione</t>
+  </si>
+  <si>
+    <t>En el login se debe validar que se haya introducido usuario y contraseña antes de llamar al servidor</t>
+  </si>
+  <si>
+    <t>Se modifica el título para que solo sean las siglas LAM</t>
+  </si>
+  <si>
+    <t>Se mete una validación en cliente en el código javascript</t>
+  </si>
+  <si>
+    <t>Las transiciones entre pantallas debe ser con slide</t>
+  </si>
+  <si>
+    <t>El header y footer deben mantenerse estáticos en las pantallas  y que el scroll sea sobre el contenido</t>
+  </si>
+  <si>
+    <t>Se modifica el método changePage para meterle el parámetro transaction:slide</t>
+  </si>
+  <si>
+    <t>Falla al actualizar un paciente que tuviera exploraciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si me meto en un paciente que tuviera 159 completas, falla en ExploracionUtilDTO.toBusiness en la línea </t>
   </si>
 </sst>
 </file>
@@ -1071,8 +1095,8 @@
   </sheetPr>
   <dimension ref="A1:O378"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1250,7 +1274,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>2</v>
       </c>
@@ -1272,62 +1296,122 @@
       <c r="G7" s="48">
         <v>41767</v>
       </c>
-      <c r="H7" s="24"/>
+      <c r="H7" s="24" t="s">
+        <v>22</v>
+      </c>
       <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J7" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
+      <c r="B8" s="22">
+        <v>41760</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="46">
+        <v>3</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="48">
+        <v>41774</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>22</v>
+      </c>
       <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J8" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
+      <c r="B9" s="22">
+        <v>41763</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="46">
+        <v>3</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="48">
+        <v>41774</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>22</v>
+      </c>
       <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J9" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
+      <c r="B10" s="22">
+        <v>41763</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="46">
+        <v>2</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="48">
+        <v>41774</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>22</v>
+      </c>
       <c r="I10" s="26"/>
       <c r="J10" s="27"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
+      <c r="C11" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="46">
+        <v>1</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="48">
+        <v>41767</v>
+      </c>
       <c r="H11" s="24"/>
       <c r="I11" s="26"/>
       <c r="J11" s="27"/>

</xml_diff>

<commit_message>
Añadido el warning e info de las faqs y metidas las fechas y descripciones para los antecedentes quirúrgicos y ortopédicos.
</commit_message>
<xml_diff>
--- a/documentacion/Documentacion_final/11 Registro de Incidencias_RI.xlsx
+++ b/documentacion/Documentacion_final/11 Registro de Incidencias_RI.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
   <si>
     <t>001</t>
   </si>
@@ -145,12 +145,6 @@
     <t>Fecha cambio de estado</t>
   </si>
   <si>
-    <t>Fecha creación Registro</t>
-  </si>
-  <si>
-    <t>dd/mm/aaaa</t>
-  </si>
-  <si>
     <t>David Llamazares Juárez</t>
   </si>
   <si>
@@ -221,6 +215,15 @@
   </si>
   <si>
     <t>Cuando se pierde la sesión y vuelve a la pantalla de login, vuelve a mostrar el mensaje de Sesión finalizada y aunque meta correctamente el usuario y la contraseña, saca el mensaje de error de usuario y/o contraseña</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>Se debe quitar el reconocimiento de voz en todas las cajas de texto de la pantalla valoracion articular muscular, puesto que todos son números y se debe cambiar el sistema para que solo permita números</t>
+  </si>
+  <si>
+    <t>Cuando hay</t>
   </si>
 </sst>
 </file>
@@ -731,70 +734,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="33">
     <dxf>
       <fill>
         <patternFill>
@@ -1390,7 +1330,7 @@
   <dimension ref="A1:O382"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1513,16 +1453,16 @@
         <v>41762</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="45">
         <v>1</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G5" s="46">
         <v>41767</v>
@@ -1532,7 +1472,7 @@
       </c>
       <c r="I5" s="47"/>
       <c r="J5" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O5" s="13" t="s">
         <v>23</v>
@@ -1546,16 +1486,16 @@
         <v>41762</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="45">
         <v>1</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="46">
         <v>41767</v>
@@ -1565,7 +1505,7 @@
       </c>
       <c r="I6" s="26"/>
       <c r="J6" s="27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
@@ -1576,16 +1516,16 @@
         <v>41762</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="45">
         <v>2</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="46">
         <v>41767</v>
@@ -1595,7 +1535,7 @@
       </c>
       <c r="I7" s="26"/>
       <c r="J7" s="27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
@@ -1606,16 +1546,16 @@
         <v>41760</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="45">
         <v>3</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G8" s="46">
         <v>41774</v>
@@ -1625,7 +1565,7 @@
       </c>
       <c r="I8" s="26"/>
       <c r="J8" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
@@ -1636,16 +1576,16 @@
         <v>41763</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="45">
         <v>3</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G9" s="46">
         <v>41774</v>
@@ -1655,7 +1595,7 @@
       </c>
       <c r="I9" s="26"/>
       <c r="J9" s="27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
@@ -1666,16 +1606,16 @@
         <v>41763</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="45">
         <v>2</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G10" s="46">
         <v>41774</v>
@@ -1694,16 +1634,16 @@
         <v>41764</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="45">
         <v>1</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G11" s="46">
         <v>41767</v>
@@ -1720,16 +1660,16 @@
         <v>41764</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" s="45">
         <v>3</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G12" s="32">
         <v>41774</v>
@@ -1742,22 +1682,22 @@
     </row>
     <row r="13" spans="1:15" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="29">
         <v>41764</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="45">
         <v>2</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G13" s="32">
         <v>41774</v>
@@ -1770,22 +1710,22 @@
     </row>
     <row r="14" spans="1:15" ht="35.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="29">
         <v>41764</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="45">
         <v>1</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G14" s="32">
         <v>41774</v>
@@ -1798,22 +1738,22 @@
     </row>
     <row r="15" spans="1:15" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="29">
         <v>41764</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="45">
         <v>1</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F15" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G15" s="32">
         <v>41774</v>
@@ -1826,22 +1766,22 @@
     </row>
     <row r="16" spans="1:15" ht="35.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="29">
         <v>41764</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="45">
         <v>1</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G16" s="32">
         <v>41774</v>
@@ -1851,27 +1791,27 @@
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" s="29">
         <v>41764</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17" s="45">
         <v>1</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F17" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G17" s="32">
         <v>41774</v>
@@ -1881,22 +1821,66 @@
       </c>
       <c r="I17" s="34"/>
       <c r="J17" s="35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="12" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="29">
+        <v>41766</v>
+      </c>
+      <c r="C18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="36"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H19" s="36"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D18" s="45">
+        <v>1</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="32">
+        <v>41774</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="34"/>
+      <c r="J18" s="35"/>
+    </row>
+    <row r="19" spans="1:10" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="29">
+        <v>41766</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="45">
+        <v>1</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="32">
+        <v>41774</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="34"/>
+      <c r="J19" s="35"/>
+    </row>
+    <row r="20" spans="1:10" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="H20" s="36"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -2988,6 +2972,28 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D5:D11">
+    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
+      <formula>$L$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="26" operator="equal">
+      <formula>$L$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
+      <formula>$L$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
+      <formula>$L$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="23" operator="equal">
+      <formula>$L$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="24" operator="equal">
+      <formula>$L$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
     <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
@@ -2998,7 +3004,7 @@
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
+  <conditionalFormatting sqref="D13">
     <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
@@ -3009,7 +3015,7 @@
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+  <conditionalFormatting sqref="D14">
     <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
@@ -3020,7 +3026,7 @@
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
+  <conditionalFormatting sqref="D15">
     <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
@@ -3031,7 +3037,7 @@
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
+  <conditionalFormatting sqref="D16">
     <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
@@ -3042,7 +3048,7 @@
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+  <conditionalFormatting sqref="D18">
     <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
@@ -3053,7 +3059,7 @@
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
+  <conditionalFormatting sqref="D19">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
@@ -3068,7 +3074,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H382">
       <formula1>$O$2:$O$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D19">
       <formula1>$L$2:$L$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -3085,21 +3091,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FB9238FD839DE1458C9EF746D117716A" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ef525560dd58d0c6ee7dc12abc3ec8e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae13a4600d56dd4d917937c2caf43faa">
     <xsd:element name="properties">
@@ -3148,16 +3139,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DDE1CEE-2F26-48C2-8103-000926593C86}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1D4419B-0089-4C39-9F39-49A51DF37CEC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3171,16 +3178,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1D4419B-0089-4C39-9F39-49A51DF37CEC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DDE1CEE-2F26-48C2-8103-000926593C86}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MAquetación de la parte servidora con bootstrap 3
</commit_message>
<xml_diff>
--- a/documentacion/Documentacion_final/11 Registro de Incidencias_RI.xlsx
+++ b/documentacion/Documentacion_final/11 Registro de Incidencias_RI.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
   <si>
     <t>001</t>
   </si>
@@ -223,7 +223,13 @@
     <t>Se debe quitar el reconocimiento de voz en todas las cajas de texto de la pantalla valoracion articular muscular, puesto que todos son números y se debe cambiar el sistema para que solo permita números</t>
   </si>
   <si>
-    <t>Cuando hay</t>
+    <t>Cambiar las transiciones entre páginas para que no actue el scrolling porque queda feo y meter un cambio de opacidad para que no se vea la recolocación mientras se muestra la pantalla</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>En las gráficas que no salga scroll horizontal, es decir, la grafica solo debe ocupar el tamaño de la pantalla y no deben aparecer los números.</t>
   </si>
 </sst>
 </file>
@@ -1329,8 +1335,8 @@
   </sheetPr>
   <dimension ref="A1:O382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1852,12 +1858,12 @@
       <c r="I18" s="34"/>
       <c r="J18" s="35"/>
     </row>
-    <row r="19" spans="1:10" ht="12.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="29">
-        <v>41766</v>
+        <v>41769</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>25</v>
@@ -1880,10 +1886,35 @@
       <c r="I19" s="34"/>
       <c r="J19" s="35"/>
     </row>
-    <row r="20" spans="1:10" ht="12" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="H20" s="36"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="35.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="29">
+        <v>41771</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="45">
+        <v>1</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="32">
+        <v>41774</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="34"/>
+      <c r="J20" s="35"/>
+    </row>
+    <row r="21" spans="1:10" ht="12" thickTop="1" x14ac:dyDescent="0.2">
       <c r="H21" s="36"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -2972,94 +3003,105 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="D5:D11">
-    <cfRule type="cellIs" dxfId="32" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="cellIs" dxfId="26" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>$L$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>$L$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>$L$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>$L$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>$L$4</formula>
     </cfRule>
@@ -3074,7 +3116,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H382">
       <formula1>$O$2:$O$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D20">
       <formula1>$L$2:$L$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -3091,6 +3133,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FB9238FD839DE1458C9EF746D117716A" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ef525560dd58d0c6ee7dc12abc3ec8e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae13a4600d56dd4d917937c2caf43faa">
     <xsd:element name="properties">
@@ -3139,32 +3196,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1D4419B-0089-4C39-9F39-49A51DF37CEC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DDE1CEE-2F26-48C2-8103-000926593C86}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3178,15 +3219,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DDE1CEE-2F26-48C2-8103-000926593C86}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1D4419B-0089-4C39-9F39-49A51DF37CEC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>